<commit_message>
resolve issue with 4 species that were missing nest site trait
</commit_message>
<xml_diff>
--- a/Results/RESULTS_TraitModelTables.xlsx
+++ b/Results/RESULTS_TraitModelTables.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t xml:space="preserve">index</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t xml:space="preserve">NestSite_High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nest site high (only)</t>
   </si>
   <si>
     <t xml:space="preserve">nest safety</t>
@@ -6605,28 +6602,28 @@
         <v>74</v>
       </c>
       <c r="E2" t="n">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
       </c>
       <c r="G2" t="n">
-        <v>1.628</v>
+        <v>1.629</v>
       </c>
       <c r="H2" t="n">
-        <v>0.198</v>
+        <v>0.203</v>
       </c>
       <c r="I2" t="n">
-        <v>8.232</v>
+        <v>8.014</v>
       </c>
       <c r="J2" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="K2" t="n">
-        <v>2.015</v>
+        <v>2.027</v>
       </c>
       <c r="L2" t="n">
-        <v>0.318</v>
+        <v>0.331</v>
       </c>
       <c r="M2"/>
     </row>
@@ -6644,28 +6641,28 @@
         <v>74</v>
       </c>
       <c r="E3" t="n">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="F3" t="s">
         <v>75</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.115</v>
+        <v>-0.112</v>
       </c>
       <c r="H3" t="n">
-        <v>0.055</v>
+        <v>0.056</v>
       </c>
       <c r="I3" t="n">
-        <v>-2.091</v>
+        <v>-2.026</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.223</v>
+        <v>-0.221</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.007</v>
+        <v>-0.004</v>
       </c>
       <c r="L3" t="n">
-        <v>0.318</v>
+        <v>0.331</v>
       </c>
       <c r="M3"/>
     </row>
@@ -6683,7 +6680,7 @@
         <v>74</v>
       </c>
       <c r="E4" t="n">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
@@ -6692,19 +6689,19 @@
         <v>-0.027</v>
       </c>
       <c r="H4" t="n">
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.215</v>
+        <v>-1.207</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.07</v>
+        <v>-0.071</v>
       </c>
       <c r="K4" t="n">
         <v>0.017</v>
       </c>
       <c r="L4" t="n">
-        <v>0.318</v>
+        <v>0.331</v>
       </c>
       <c r="M4"/>
     </row>
@@ -6956,7 +6953,7 @@
         <v>76</v>
       </c>
       <c r="E11" t="n">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -6965,19 +6962,19 @@
         <v>1.632</v>
       </c>
       <c r="H11" t="n">
-        <v>0.157</v>
+        <v>0.159</v>
       </c>
       <c r="I11" t="n">
-        <v>10.371</v>
+        <v>10.256</v>
       </c>
       <c r="J11" t="n">
-        <v>1.323</v>
+        <v>1.32</v>
       </c>
       <c r="K11" t="n">
-        <v>1.94</v>
+        <v>1.944</v>
       </c>
       <c r="L11" t="n">
-        <v>0.146</v>
+        <v>0.148</v>
       </c>
       <c r="M11"/>
     </row>
@@ -6995,28 +6992,28 @@
         <v>76</v>
       </c>
       <c r="E12" t="n">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="F12" t="s">
         <v>75</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.223</v>
+        <v>-0.22</v>
       </c>
       <c r="H12" t="n">
         <v>0.068</v>
       </c>
       <c r="I12" t="n">
-        <v>-3.297</v>
+        <v>-3.226</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.355</v>
+        <v>-0.354</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.09</v>
+        <v>-0.086</v>
       </c>
       <c r="L12" t="n">
-        <v>0.146</v>
+        <v>0.148</v>
       </c>
       <c r="M12"/>
     </row>
@@ -7034,28 +7031,28 @@
         <v>76</v>
       </c>
       <c r="E13" t="n">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.023</v>
+        <v>-0.024</v>
       </c>
       <c r="H13" t="n">
-        <v>0.021</v>
+        <v>0.022</v>
       </c>
       <c r="I13" t="n">
-        <v>-1.087</v>
+        <v>-1.09</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.065</v>
+        <v>-0.066</v>
       </c>
       <c r="K13" t="n">
         <v>0.019</v>
       </c>
       <c r="L13" t="n">
-        <v>0.146</v>
+        <v>0.148</v>
       </c>
       <c r="M13"/>
     </row>
@@ -7658,28 +7655,28 @@
         <v>79</v>
       </c>
       <c r="E29" t="n">
-        <v>575</v>
+        <v>766</v>
       </c>
       <c r="F29" t="s">
         <v>17</v>
       </c>
       <c r="G29" t="n">
-        <v>1.424</v>
+        <v>1.633</v>
       </c>
       <c r="H29" t="n">
-        <v>0.164</v>
+        <v>0.229</v>
       </c>
       <c r="I29" t="n">
-        <v>8.67</v>
+        <v>7.118</v>
       </c>
       <c r="J29" t="n">
-        <v>1.102</v>
+        <v>1.183</v>
       </c>
       <c r="K29" t="n">
-        <v>1.746</v>
+        <v>2.082</v>
       </c>
       <c r="L29" t="n">
-        <v>0.143</v>
+        <v>0.393</v>
       </c>
       <c r="M29"/>
     </row>
@@ -7697,28 +7694,28 @@
         <v>79</v>
       </c>
       <c r="E30" t="n">
-        <v>575</v>
+        <v>766</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G30" t="n">
-        <v>0.215</v>
+        <v>0.013</v>
       </c>
       <c r="H30" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.466</v>
+      </c>
+      <c r="J30" t="n">
+        <v>-0.041</v>
+      </c>
+      <c r="K30" t="n">
         <v>0.067</v>
       </c>
-      <c r="I30" t="n">
-        <v>3.188</v>
-      </c>
-      <c r="J30" t="n">
-        <v>0.083</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0.346</v>
-      </c>
       <c r="L30" t="n">
-        <v>0.143</v>
+        <v>0.393</v>
       </c>
       <c r="M30"/>
     </row>
@@ -7736,28 +7733,28 @@
         <v>79</v>
       </c>
       <c r="E31" t="n">
-        <v>575</v>
+        <v>766</v>
       </c>
       <c r="F31" t="s">
         <v>18</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.024</v>
+        <v>-0.043</v>
       </c>
       <c r="H31" t="n">
-        <v>0.021</v>
+        <v>0.023</v>
       </c>
       <c r="I31" t="n">
-        <v>-1.12</v>
+        <v>-1.839</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.066</v>
+        <v>-0.088</v>
       </c>
       <c r="K31" t="n">
-        <v>0.018</v>
+        <v>0.003</v>
       </c>
       <c r="L31" t="n">
-        <v>0.143</v>
+        <v>0.393</v>
       </c>
       <c r="M31"/>
     </row>
@@ -7775,28 +7772,28 @@
         <v>79</v>
       </c>
       <c r="E32" t="n">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F32" t="s">
         <v>17</v>
       </c>
       <c r="G32" t="n">
-        <v>-1.118</v>
+        <v>-1.223</v>
       </c>
       <c r="H32" t="n">
-        <v>0.765</v>
+        <v>0.789</v>
       </c>
       <c r="I32" t="n">
-        <v>-1.463</v>
+        <v>-1.55</v>
       </c>
       <c r="J32" t="n">
-        <v>-2.617</v>
+        <v>-2.768</v>
       </c>
       <c r="K32" t="n">
-        <v>0.38</v>
+        <v>0.323</v>
       </c>
       <c r="L32" t="n">
-        <v>0.3</v>
+        <v>0.351</v>
       </c>
       <c r="M32"/>
     </row>
@@ -7814,28 +7811,28 @@
         <v>79</v>
       </c>
       <c r="E33" t="n">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G33" t="n">
-        <v>0.729</v>
+        <v>0.177</v>
       </c>
       <c r="H33" t="n">
-        <v>0.354</v>
+        <v>0.141</v>
       </c>
       <c r="I33" t="n">
-        <v>2.06</v>
+        <v>1.259</v>
       </c>
       <c r="J33" t="n">
-        <v>0.035</v>
+        <v>-0.099</v>
       </c>
       <c r="K33" t="n">
-        <v>1.422</v>
+        <v>0.453</v>
       </c>
       <c r="L33" t="n">
-        <v>0.3</v>
+        <v>0.351</v>
       </c>
       <c r="M33"/>
     </row>
@@ -7853,28 +7850,28 @@
         <v>79</v>
       </c>
       <c r="E34" t="n">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F34" t="s">
         <v>18</v>
       </c>
       <c r="G34" t="n">
-        <v>0.125</v>
+        <v>0.159</v>
       </c>
       <c r="H34" t="n">
-        <v>0.108</v>
+        <v>0.101</v>
       </c>
       <c r="I34" t="n">
-        <v>1.156</v>
+        <v>1.572</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.087</v>
+        <v>-0.039</v>
       </c>
       <c r="K34" t="n">
-        <v>0.338</v>
+        <v>0.358</v>
       </c>
       <c r="L34" t="n">
-        <v>0.3</v>
+        <v>0.351</v>
       </c>
       <c r="M34"/>
     </row>
@@ -7892,29 +7889,29 @@
         <v>79</v>
       </c>
       <c r="E35" t="n">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="F35" t="s">
         <v>17</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.248</v>
+        <v>-0.86</v>
       </c>
       <c r="H35" t="n">
-        <v>0.287</v>
+        <v>0.21</v>
       </c>
       <c r="I35" t="n">
-        <v>-4.345</v>
+        <v>-4.1</v>
       </c>
       <c r="J35" t="n">
-        <v>-1.895</v>
+        <v>-1.359</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.57</v>
+        <v>-0.371</v>
       </c>
       <c r="L35"/>
       <c r="M35" t="n">
-        <v>0.558</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="36">
@@ -7931,29 +7928,29 @@
         <v>79</v>
       </c>
       <c r="E36" t="n">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="F36" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G36" t="n">
-        <v>0.986</v>
+        <v>0.455</v>
       </c>
       <c r="H36" t="n">
-        <v>0.519</v>
+        <v>0.205</v>
       </c>
       <c r="I36" t="n">
-        <v>1.901</v>
+        <v>2.222</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.403</v>
+        <v>-0.004</v>
       </c>
       <c r="K36" t="n">
-        <v>2.094</v>
+        <v>0.966</v>
       </c>
       <c r="L36"/>
       <c r="M36" t="n">
-        <v>0.558</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="37">
@@ -7970,29 +7967,29 @@
         <v>79</v>
       </c>
       <c r="E37" t="n">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="F37" t="s">
         <v>22</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.036</v>
+        <v>0.139</v>
       </c>
       <c r="H37" t="n">
-        <v>0.244</v>
+        <v>0.213</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.149</v>
+        <v>0.653</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.578</v>
+        <v>-0.321</v>
       </c>
       <c r="K37" t="n">
-        <v>0.58</v>
+        <v>0.645</v>
       </c>
       <c r="L37"/>
       <c r="M37" t="n">
-        <v>0.558</v>
+        <v>0.548</v>
       </c>
     </row>
     <row r="38">
@@ -8006,31 +8003,31 @@
         <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E38" t="n">
-        <v>766</v>
+        <v>733</v>
       </c>
       <c r="F38" t="s">
         <v>17</v>
       </c>
       <c r="G38" t="n">
-        <v>1.633</v>
+        <v>1.529</v>
       </c>
       <c r="H38" t="n">
-        <v>0.229</v>
+        <v>0.217</v>
       </c>
       <c r="I38" t="n">
-        <v>7.118</v>
+        <v>7.056</v>
       </c>
       <c r="J38" t="n">
-        <v>1.183</v>
+        <v>1.104</v>
       </c>
       <c r="K38" t="n">
-        <v>2.082</v>
+        <v>1.953</v>
       </c>
       <c r="L38" t="n">
-        <v>0.393</v>
+        <v>0.372</v>
       </c>
       <c r="M38"/>
     </row>
@@ -8045,31 +8042,31 @@
         <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E39" t="n">
-        <v>766</v>
+        <v>733</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G39" t="n">
-        <v>0.013</v>
+        <v>0.034</v>
       </c>
       <c r="H39" t="n">
-        <v>0.028</v>
+        <v>0.078</v>
       </c>
       <c r="I39" t="n">
-        <v>0.466</v>
+        <v>0.435</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.041</v>
+        <v>-0.118</v>
       </c>
       <c r="K39" t="n">
-        <v>0.067</v>
+        <v>0.186</v>
       </c>
       <c r="L39" t="n">
-        <v>0.393</v>
+        <v>0.372</v>
       </c>
       <c r="M39"/>
     </row>
@@ -8084,31 +8081,31 @@
         <v>73</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E40" t="n">
-        <v>766</v>
+        <v>733</v>
       </c>
       <c r="F40" t="s">
         <v>18</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.043</v>
+        <v>-0.025</v>
       </c>
       <c r="H40" t="n">
         <v>0.023</v>
       </c>
       <c r="I40" t="n">
-        <v>-1.839</v>
+        <v>-1.062</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.088</v>
+        <v>-0.07</v>
       </c>
       <c r="K40" t="n">
-        <v>0.003</v>
+        <v>0.021</v>
       </c>
       <c r="L40" t="n">
-        <v>0.393</v>
+        <v>0.372</v>
       </c>
       <c r="M40"/>
     </row>
@@ -8123,31 +8120,31 @@
         <v>73</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E41" t="n">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F41" t="s">
         <v>17</v>
       </c>
       <c r="G41" t="n">
-        <v>-1.223</v>
+        <v>-0.904</v>
       </c>
       <c r="H41" t="n">
-        <v>0.789</v>
+        <v>0.796</v>
       </c>
       <c r="I41" t="n">
-        <v>-1.55</v>
+        <v>-1.136</v>
       </c>
       <c r="J41" t="n">
-        <v>-2.768</v>
+        <v>-2.464</v>
       </c>
       <c r="K41" t="n">
-        <v>0.323</v>
+        <v>0.656</v>
       </c>
       <c r="L41" t="n">
-        <v>0.351</v>
+        <v>0.32</v>
       </c>
       <c r="M41"/>
     </row>
@@ -8162,31 +8159,31 @@
         <v>73</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E42" t="n">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G42" t="n">
-        <v>0.177</v>
+        <v>-0.22</v>
       </c>
       <c r="H42" t="n">
-        <v>0.141</v>
+        <v>0.491</v>
       </c>
       <c r="I42" t="n">
-        <v>1.259</v>
+        <v>-0.447</v>
       </c>
       <c r="J42" t="n">
-        <v>-0.099</v>
+        <v>-1.183</v>
       </c>
       <c r="K42" t="n">
-        <v>0.453</v>
+        <v>0.743</v>
       </c>
       <c r="L42" t="n">
-        <v>0.351</v>
+        <v>0.32</v>
       </c>
       <c r="M42"/>
     </row>
@@ -8201,384 +8198,33 @@
         <v>73</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E43" t="n">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F43" t="s">
         <v>18</v>
       </c>
       <c r="G43" t="n">
-        <v>0.159</v>
+        <v>0.186</v>
       </c>
       <c r="H43" t="n">
-        <v>0.101</v>
+        <v>0.108</v>
       </c>
       <c r="I43" t="n">
-        <v>1.572</v>
+        <v>1.72</v>
       </c>
       <c r="J43" t="n">
-        <v>-0.039</v>
+        <v>-0.026</v>
       </c>
       <c r="K43" t="n">
-        <v>0.358</v>
+        <v>0.397</v>
       </c>
       <c r="L43" t="n">
-        <v>0.351</v>
+        <v>0.32</v>
       </c>
       <c r="M43"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" t="n">
-        <v>129</v>
-      </c>
-      <c r="F44" t="s">
-        <v>17</v>
-      </c>
-      <c r="G44" t="n">
-        <v>-0.86</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="I44" t="n">
-        <v>-4.1</v>
-      </c>
-      <c r="J44" t="n">
-        <v>-1.359</v>
-      </c>
-      <c r="K44" t="n">
-        <v>-0.371</v>
-      </c>
-      <c r="L44"/>
-      <c r="M44" t="n">
-        <v>0.548</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" t="n">
-        <v>129</v>
-      </c>
-      <c r="F45" t="s">
-        <v>82</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0.455</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0.205</v>
-      </c>
-      <c r="I45" t="n">
-        <v>2.222</v>
-      </c>
-      <c r="J45" t="n">
-        <v>-0.004</v>
-      </c>
-      <c r="K45" t="n">
-        <v>0.966</v>
-      </c>
-      <c r="L45"/>
-      <c r="M45" t="n">
-        <v>0.548</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" t="s">
-        <v>73</v>
-      </c>
-      <c r="D46" t="s">
-        <v>80</v>
-      </c>
-      <c r="E46" t="n">
-        <v>129</v>
-      </c>
-      <c r="F46" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.139</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0.213</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0.653</v>
-      </c>
-      <c r="J46" t="n">
-        <v>-0.321</v>
-      </c>
-      <c r="K46" t="n">
-        <v>0.645</v>
-      </c>
-      <c r="L46"/>
-      <c r="M46" t="n">
-        <v>0.548</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" t="s">
-        <v>83</v>
-      </c>
-      <c r="E47" t="n">
-        <v>733</v>
-      </c>
-      <c r="F47" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" t="n">
-        <v>1.529</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0.217</v>
-      </c>
-      <c r="I47" t="n">
-        <v>7.056</v>
-      </c>
-      <c r="J47" t="n">
-        <v>1.104</v>
-      </c>
-      <c r="K47" t="n">
-        <v>1.953</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0.372</v>
-      </c>
-      <c r="M47"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" t="s">
-        <v>73</v>
-      </c>
-      <c r="D48" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" t="n">
-        <v>733</v>
-      </c>
-      <c r="F48" t="s">
-        <v>84</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.034</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0.078</v>
-      </c>
-      <c r="I48" t="n">
-        <v>0.435</v>
-      </c>
-      <c r="J48" t="n">
-        <v>-0.118</v>
-      </c>
-      <c r="K48" t="n">
-        <v>0.186</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0.372</v>
-      </c>
-      <c r="M48"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" t="n">
-        <v>733</v>
-      </c>
-      <c r="F49" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" t="n">
-        <v>-0.025</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0.023</v>
-      </c>
-      <c r="I49" t="n">
-        <v>-1.062</v>
-      </c>
-      <c r="J49" t="n">
-        <v>-0.07</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0.021</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0.372</v>
-      </c>
-      <c r="M49"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" t="s">
-        <v>83</v>
-      </c>
-      <c r="E50" t="n">
-        <v>117</v>
-      </c>
-      <c r="F50" t="s">
-        <v>17</v>
-      </c>
-      <c r="G50" t="n">
-        <v>-0.904</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.796</v>
-      </c>
-      <c r="I50" t="n">
-        <v>-1.136</v>
-      </c>
-      <c r="J50" t="n">
-        <v>-2.464</v>
-      </c>
-      <c r="K50" t="n">
-        <v>0.656</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="M50"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" t="s">
-        <v>83</v>
-      </c>
-      <c r="E51" t="n">
-        <v>117</v>
-      </c>
-      <c r="F51" t="s">
-        <v>84</v>
-      </c>
-      <c r="G51" t="n">
-        <v>-0.22</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0.491</v>
-      </c>
-      <c r="I51" t="n">
-        <v>-0.447</v>
-      </c>
-      <c r="J51" t="n">
-        <v>-1.183</v>
-      </c>
-      <c r="K51" t="n">
-        <v>0.743</v>
-      </c>
-      <c r="L51" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="M51"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" t="s">
-        <v>83</v>
-      </c>
-      <c r="E52" t="n">
-        <v>117</v>
-      </c>
-      <c r="F52" t="s">
-        <v>18</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0.186</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0.108</v>
-      </c>
-      <c r="I52" t="n">
-        <v>1.72</v>
-      </c>
-      <c r="J52" t="n">
-        <v>-0.026</v>
-      </c>
-      <c r="K52" t="n">
-        <v>0.397</v>
-      </c>
-      <c r="L52" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="M52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update nest site high UAI model
</commit_message>
<xml_diff>
--- a/Results/RESULTS_TraitModelTables.xlsx
+++ b/Results/RESULTS_TraitModelTables.xlsx
@@ -7304,28 +7304,28 @@
         <v>77</v>
       </c>
       <c r="E20" t="n">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
       </c>
       <c r="G20" t="n">
-        <v>1.453</v>
+        <v>1.438</v>
       </c>
       <c r="H20" t="n">
-        <v>0.202</v>
+        <v>0.208</v>
       </c>
       <c r="I20" t="n">
-        <v>7.196</v>
+        <v>6.927</v>
       </c>
       <c r="J20" t="n">
-        <v>1.058</v>
+        <v>1.031</v>
       </c>
       <c r="K20" t="n">
-        <v>1.849</v>
+        <v>1.845</v>
       </c>
       <c r="L20" t="n">
-        <v>0.321</v>
+        <v>0.333</v>
       </c>
       <c r="M20"/>
     </row>
@@ -7343,28 +7343,28 @@
         <v>77</v>
       </c>
       <c r="E21" t="n">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="F21" t="s">
         <v>78</v>
       </c>
       <c r="G21" t="n">
-        <v>0.177</v>
+        <v>0.181</v>
       </c>
       <c r="H21" t="n">
         <v>0.051</v>
       </c>
       <c r="I21" t="n">
-        <v>3.489</v>
+        <v>3.528</v>
       </c>
       <c r="J21" t="n">
-        <v>0.077</v>
+        <v>0.08</v>
       </c>
       <c r="K21" t="n">
-        <v>0.276</v>
+        <v>0.281</v>
       </c>
       <c r="L21" t="n">
-        <v>0.321</v>
+        <v>0.333</v>
       </c>
       <c r="M21"/>
     </row>
@@ -7382,7 +7382,7 @@
         <v>77</v>
       </c>
       <c r="E22" t="n">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="F22" t="s">
         <v>18</v>
@@ -7394,16 +7394,16 @@
         <v>0.022</v>
       </c>
       <c r="I22" t="n">
-        <v>-1.293</v>
+        <v>-1.246</v>
       </c>
       <c r="J22" t="n">
         <v>-0.071</v>
       </c>
       <c r="K22" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="L22" t="n">
-        <v>0.321</v>
+        <v>0.333</v>
       </c>
       <c r="M22"/>
     </row>

</xml_diff>